<commit_message>
major model revamp with pickups
</commit_message>
<xml_diff>
--- a/data/matrix.xlsx
+++ b/data/matrix.xlsx
@@ -590,88 +590,88 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>42612</v>
+        <v>40628</v>
       </c>
       <c r="D2" t="n">
-        <v>149364</v>
+        <v>142865</v>
       </c>
       <c r="E2" t="n">
-        <v>32046</v>
+        <v>27451</v>
       </c>
       <c r="F2" t="n">
-        <v>8764</v>
+        <v>8765</v>
       </c>
       <c r="G2" t="n">
-        <v>50463</v>
+        <v>48829</v>
       </c>
       <c r="H2" t="n">
-        <v>65099</v>
+        <v>63030</v>
       </c>
       <c r="I2" t="n">
-        <v>22821</v>
+        <v>17091</v>
       </c>
       <c r="J2" t="n">
-        <v>22628</v>
+        <v>20063</v>
       </c>
       <c r="K2" t="n">
         <v>6373</v>
       </c>
       <c r="L2" t="n">
-        <v>28915</v>
+        <v>23703</v>
       </c>
       <c r="M2" t="n">
-        <v>29983</v>
+        <v>25957</v>
       </c>
       <c r="N2" t="n">
-        <v>72846</v>
+        <v>66957</v>
       </c>
       <c r="O2" t="n">
-        <v>24764</v>
+        <v>22196</v>
       </c>
       <c r="P2" t="n">
-        <v>29956</v>
+        <v>28246</v>
       </c>
       <c r="Q2" t="n">
-        <v>113021</v>
+        <v>111389</v>
       </c>
       <c r="R2" t="n">
-        <v>26879</v>
+        <v>23602</v>
       </c>
       <c r="S2" t="n">
-        <v>20735</v>
+        <v>17633</v>
       </c>
       <c r="T2" t="n">
-        <v>19495</v>
+        <v>16394</v>
       </c>
       <c r="U2" t="n">
-        <v>18781</v>
+        <v>13674</v>
       </c>
       <c r="V2" t="n">
-        <v>62498</v>
+        <v>56824</v>
       </c>
       <c r="W2" t="n">
-        <v>46522</v>
+        <v>41657</v>
       </c>
       <c r="X2" t="n">
-        <v>100878</v>
+        <v>99244</v>
       </c>
       <c r="Y2" t="n">
-        <v>86099</v>
+        <v>84467</v>
       </c>
       <c r="Z2" t="n">
-        <v>10221</v>
+        <v>8278</v>
       </c>
       <c r="AA2" t="n">
-        <v>14019</v>
+        <v>12287</v>
       </c>
       <c r="AB2" t="n">
-        <v>11723</v>
+        <v>8601</v>
       </c>
       <c r="AC2" t="n">
-        <v>18525</v>
+        <v>15423</v>
       </c>
       <c r="AD2" t="n">
-        <v>41929</v>
+        <v>39362</v>
       </c>
     </row>
     <row r="3">
@@ -681,91 +681,91 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>42607</v>
+        <v>40220</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>127022</v>
+        <v>122154</v>
       </c>
       <c r="E3" t="n">
-        <v>72673</v>
+        <v>66826</v>
       </c>
       <c r="F3" t="n">
-        <v>41486</v>
+        <v>40675</v>
       </c>
       <c r="G3" t="n">
-        <v>28121</v>
+        <v>27961</v>
       </c>
       <c r="H3" t="n">
-        <v>42757</v>
+        <v>42125</v>
       </c>
       <c r="I3" t="n">
-        <v>28469</v>
+        <v>28468</v>
       </c>
       <c r="J3" t="n">
-        <v>28216</v>
+        <v>26790</v>
       </c>
       <c r="K3" t="n">
         <v>44456</v>
       </c>
       <c r="L3" t="n">
-        <v>36476</v>
+        <v>33763</v>
       </c>
       <c r="M3" t="n">
-        <v>64880</v>
+        <v>64040</v>
       </c>
       <c r="N3" t="n">
-        <v>63822</v>
+        <v>62794</v>
       </c>
       <c r="O3" t="n">
-        <v>49849</v>
+        <v>41540</v>
       </c>
       <c r="P3" t="n">
-        <v>55041</v>
+        <v>51388</v>
       </c>
       <c r="Q3" t="n">
-        <v>90679</v>
+        <v>90678</v>
       </c>
       <c r="R3" t="n">
-        <v>28554</v>
+        <v>22450</v>
       </c>
       <c r="S3" t="n">
-        <v>45820</v>
+        <v>43464</v>
       </c>
       <c r="T3" t="n">
-        <v>34659</v>
+        <v>34658</v>
       </c>
       <c r="U3" t="n">
-        <v>26791</v>
+        <v>26793</v>
       </c>
       <c r="V3" t="n">
-        <v>53690</v>
+        <v>53331</v>
       </c>
       <c r="W3" t="n">
-        <v>35204</v>
+        <v>35202</v>
       </c>
       <c r="X3" t="n">
-        <v>78536</v>
+        <v>78533</v>
       </c>
       <c r="Y3" t="n">
-        <v>63757</v>
+        <v>63756</v>
       </c>
       <c r="Z3" t="n">
         <v>34713</v>
       </c>
       <c r="AA3" t="n">
-        <v>39837</v>
+        <v>32345</v>
       </c>
       <c r="AB3" t="n">
         <v>32936</v>
       </c>
       <c r="AC3" t="n">
-        <v>34908</v>
+        <v>34907</v>
       </c>
       <c r="AD3" t="n">
-        <v>25824</v>
+        <v>25825</v>
       </c>
     </row>
     <row r="4">
@@ -775,91 +775,91 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>149323</v>
+        <v>141932</v>
       </c>
       <c r="C4" t="n">
-        <v>126804</v>
+        <v>119381</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>179388</v>
+        <v>168538</v>
       </c>
       <c r="F4" t="n">
-        <v>148201</v>
+        <v>142387</v>
       </c>
       <c r="G4" t="n">
-        <v>102657</v>
+        <v>97167</v>
       </c>
       <c r="H4" t="n">
-        <v>92814</v>
+        <v>82620</v>
       </c>
       <c r="I4" t="n">
-        <v>130750</v>
+        <v>125659</v>
       </c>
       <c r="J4" t="n">
-        <v>151121</v>
+        <v>145089</v>
       </c>
       <c r="K4" t="n">
-        <v>151171</v>
+        <v>146168</v>
       </c>
       <c r="L4" t="n">
-        <v>134321</v>
+        <v>124976</v>
       </c>
       <c r="M4" t="n">
-        <v>171595</v>
+        <v>165752</v>
       </c>
       <c r="N4" t="n">
-        <v>86451</v>
+        <v>86452</v>
       </c>
       <c r="O4" t="n">
-        <v>156564</v>
+        <v>132835</v>
       </c>
       <c r="P4" t="n">
-        <v>161757</v>
+        <v>132661</v>
       </c>
       <c r="Q4" t="n">
-        <v>39813</v>
+        <v>39812</v>
       </c>
       <c r="R4" t="n">
-        <v>124256</v>
+        <v>119164</v>
       </c>
       <c r="S4" t="n">
-        <v>152535</v>
+        <v>137178</v>
       </c>
       <c r="T4" t="n">
-        <v>135496</v>
+        <v>130404</v>
       </c>
       <c r="U4" t="n">
-        <v>133507</v>
+        <v>128505</v>
       </c>
       <c r="V4" t="n">
-        <v>194099</v>
+        <v>172712</v>
       </c>
       <c r="W4" t="n">
-        <v>116420</v>
+        <v>106570</v>
       </c>
       <c r="X4" t="n">
-        <v>47744</v>
+        <v>47743</v>
       </c>
       <c r="Y4" t="n">
-        <v>77479</v>
+        <v>58366</v>
       </c>
       <c r="Z4" t="n">
-        <v>141428</v>
+        <v>136425</v>
       </c>
       <c r="AA4" t="n">
-        <v>146552</v>
+        <v>141548</v>
       </c>
       <c r="AB4" t="n">
-        <v>139651</v>
+        <v>134648</v>
       </c>
       <c r="AC4" t="n">
-        <v>137440</v>
+        <v>132348</v>
       </c>
       <c r="AD4" t="n">
-        <v>170553</v>
+        <v>145206</v>
       </c>
     </row>
     <row r="5">
@@ -869,91 +869,91 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>30739</v>
+        <v>27465</v>
       </c>
       <c r="C5" t="n">
-        <v>70775</v>
+        <v>67617</v>
       </c>
       <c r="D5" t="n">
-        <v>177527</v>
+        <v>169537</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>39472</v>
+        <v>34918</v>
       </c>
       <c r="G5" t="n">
-        <v>78626</v>
+        <v>75501</v>
       </c>
       <c r="H5" t="n">
-        <v>93262</v>
+        <v>89702</v>
       </c>
       <c r="I5" t="n">
-        <v>50984</v>
+        <v>43763</v>
       </c>
       <c r="J5" t="n">
-        <v>43882</v>
+        <v>43549</v>
       </c>
       <c r="K5" t="n">
-        <v>34931</v>
+        <v>25566</v>
       </c>
       <c r="L5" t="n">
-        <v>57078</v>
+        <v>50280</v>
       </c>
       <c r="M5" t="n">
         <v>22093</v>
       </c>
       <c r="N5" t="n">
-        <v>101010</v>
+        <v>93652</v>
       </c>
       <c r="O5" t="n">
-        <v>52927</v>
+        <v>48919</v>
       </c>
       <c r="P5" t="n">
-        <v>58120</v>
+        <v>50317</v>
       </c>
       <c r="Q5" t="n">
-        <v>141184</v>
+        <v>138061</v>
       </c>
       <c r="R5" t="n">
-        <v>55042</v>
+        <v>50121</v>
       </c>
       <c r="S5" t="n">
-        <v>48898</v>
+        <v>44891</v>
       </c>
       <c r="T5" t="n">
-        <v>47658</v>
+        <v>43089</v>
       </c>
       <c r="U5" t="n">
-        <v>46944</v>
+        <v>40193</v>
       </c>
       <c r="V5" t="n">
-        <v>62387</v>
+        <v>58419</v>
       </c>
       <c r="W5" t="n">
-        <v>74685</v>
+        <v>67810</v>
       </c>
       <c r="X5" t="n">
-        <v>129041</v>
+        <v>125916</v>
       </c>
       <c r="Y5" t="n">
-        <v>114262</v>
+        <v>111139</v>
       </c>
       <c r="Z5" t="n">
-        <v>38384</v>
+        <v>34376</v>
       </c>
       <c r="AA5" t="n">
-        <v>35274</v>
+        <v>35273</v>
       </c>
       <c r="AB5" t="n">
-        <v>39887</v>
+        <v>35120</v>
       </c>
       <c r="AC5" t="n">
-        <v>46689</v>
+        <v>42118</v>
       </c>
       <c r="AD5" t="n">
-        <v>63184</v>
+        <v>56423</v>
       </c>
     </row>
     <row r="6">
@@ -963,91 +963,91 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9209</v>
+        <v>9157</v>
       </c>
       <c r="C6" t="n">
-        <v>41003</v>
+        <v>41004</v>
       </c>
       <c r="D6" t="n">
-        <v>147755</v>
+        <v>142302</v>
       </c>
       <c r="E6" t="n">
-        <v>41559</v>
+        <v>36322</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>48854</v>
+        <v>48266</v>
       </c>
       <c r="H6" t="n">
-        <v>63490</v>
+        <v>62761</v>
       </c>
       <c r="I6" t="n">
-        <v>17188</v>
+        <v>16528</v>
       </c>
       <c r="J6" t="n">
-        <v>27833</v>
+        <v>23450</v>
       </c>
       <c r="K6" t="n">
-        <v>13831</v>
+        <v>13347</v>
       </c>
       <c r="L6" t="n">
-        <v>24103</v>
+        <v>21534</v>
       </c>
       <c r="M6" t="n">
-        <v>34255</v>
+        <v>26941</v>
       </c>
       <c r="N6" t="n">
-        <v>68035</v>
+        <v>64788</v>
       </c>
       <c r="O6" t="n">
-        <v>19953</v>
+        <v>17601</v>
       </c>
       <c r="P6" t="n">
-        <v>19681</v>
+        <v>19682</v>
       </c>
       <c r="Q6" t="n">
-        <v>111412</v>
+        <v>110826</v>
       </c>
       <c r="R6" t="n">
-        <v>25271</v>
+        <v>25040</v>
       </c>
       <c r="S6" t="n">
-        <v>12408</v>
+        <v>12407</v>
       </c>
       <c r="T6" t="n">
-        <v>14684</v>
+        <v>14225</v>
       </c>
       <c r="U6" t="n">
-        <v>17172</v>
+        <v>15112</v>
       </c>
       <c r="V6" t="n">
-        <v>70811</v>
+        <v>60230</v>
       </c>
       <c r="W6" t="n">
-        <v>44913</v>
+        <v>38946</v>
       </c>
       <c r="X6" t="n">
-        <v>99270</v>
+        <v>98681</v>
       </c>
       <c r="Y6" t="n">
-        <v>84490</v>
+        <v>83904</v>
       </c>
       <c r="Z6" t="n">
-        <v>6537</v>
+        <v>6538</v>
       </c>
       <c r="AA6" t="n">
-        <v>23532</v>
+        <v>16499</v>
       </c>
       <c r="AB6" t="n">
-        <v>9981</v>
+        <v>8070</v>
       </c>
       <c r="AC6" t="n">
-        <v>13714</v>
+        <v>13254</v>
       </c>
       <c r="AD6" t="n">
-        <v>47265</v>
+        <v>42749</v>
       </c>
     </row>
     <row r="7">
@@ -1057,91 +1057,91 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>50070</v>
+        <v>47682</v>
       </c>
       <c r="C7" t="n">
-        <v>27551</v>
+        <v>26146</v>
       </c>
       <c r="D7" t="n">
-        <v>102929</v>
+        <v>96474</v>
       </c>
       <c r="E7" t="n">
-        <v>80135</v>
+        <v>74288</v>
       </c>
       <c r="F7" t="n">
-        <v>48949</v>
+        <v>48137</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>14772</v>
+        <v>14773</v>
       </c>
       <c r="I7" t="n">
         <v>31497</v>
       </c>
       <c r="J7" t="n">
-        <v>51868</v>
+        <v>47922</v>
       </c>
       <c r="K7" t="n">
-        <v>51919</v>
+        <v>51918</v>
       </c>
       <c r="L7" t="n">
-        <v>35068</v>
+        <v>34761</v>
       </c>
       <c r="M7" t="n">
-        <v>72343</v>
+        <v>71502</v>
       </c>
       <c r="N7" t="n">
         <v>39284</v>
       </c>
       <c r="O7" t="n">
-        <v>57312</v>
+        <v>42620</v>
       </c>
       <c r="P7" t="n">
-        <v>62504</v>
+        <v>52693</v>
       </c>
       <c r="Q7" t="n">
-        <v>66586</v>
+        <v>66587</v>
       </c>
       <c r="R7" t="n">
-        <v>25003</v>
+        <v>25002</v>
       </c>
       <c r="S7" t="n">
-        <v>53283</v>
+        <v>44769</v>
       </c>
       <c r="T7" t="n">
-        <v>36243</v>
+        <v>36242</v>
       </c>
       <c r="U7" t="n">
-        <v>34254</v>
+        <v>34255</v>
       </c>
       <c r="V7" t="n">
-        <v>94846</v>
+        <v>79477</v>
       </c>
       <c r="W7" t="n">
-        <v>18189</v>
+        <v>18188</v>
       </c>
       <c r="X7" t="n">
-        <v>54444</v>
+        <v>53227</v>
       </c>
       <c r="Y7" t="n">
-        <v>39664</v>
+        <v>38076</v>
       </c>
       <c r="Z7" t="n">
-        <v>42176</v>
+        <v>42175</v>
       </c>
       <c r="AA7" t="n">
-        <v>47299</v>
+        <v>47298</v>
       </c>
       <c r="AB7" t="n">
         <v>40398</v>
       </c>
       <c r="AC7" t="n">
-        <v>38187</v>
+        <v>38186</v>
       </c>
       <c r="AD7" t="n">
-        <v>71300</v>
+        <v>51971</v>
       </c>
     </row>
     <row r="8">
@@ -1151,19 +1151,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>64880</v>
+        <v>62491</v>
       </c>
       <c r="C8" t="n">
-        <v>42361</v>
+        <v>40454</v>
       </c>
       <c r="D8" t="n">
-        <v>93279</v>
+        <v>82623</v>
       </c>
       <c r="E8" t="n">
-        <v>94945</v>
+        <v>89097</v>
       </c>
       <c r="F8" t="n">
-        <v>63758</v>
+        <v>62946</v>
       </c>
       <c r="G8" t="n">
         <v>15457</v>
@@ -1172,70 +1172,70 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>46307</v>
+        <v>46023</v>
       </c>
       <c r="J8" t="n">
-        <v>66678</v>
+        <v>62732</v>
       </c>
       <c r="K8" t="n">
-        <v>66728</v>
+        <v>66727</v>
       </c>
       <c r="L8" t="n">
-        <v>49878</v>
+        <v>47274</v>
       </c>
       <c r="M8" t="n">
-        <v>87152</v>
+        <v>86311</v>
       </c>
       <c r="N8" t="n">
-        <v>37589</v>
+        <v>37587</v>
       </c>
       <c r="O8" t="n">
-        <v>72121</v>
+        <v>55133</v>
       </c>
       <c r="P8" t="n">
-        <v>77314</v>
+        <v>63895</v>
       </c>
       <c r="Q8" t="n">
-        <v>56936</v>
+        <v>55026</v>
       </c>
       <c r="R8" t="n">
         <v>39812</v>
       </c>
       <c r="S8" t="n">
-        <v>68092</v>
+        <v>59295</v>
       </c>
       <c r="T8" t="n">
-        <v>51053</v>
+        <v>50768</v>
       </c>
       <c r="U8" t="n">
         <v>49064</v>
       </c>
       <c r="V8" t="n">
-        <v>109656</v>
+        <v>93785</v>
       </c>
       <c r="W8" t="n">
-        <v>28869</v>
+        <v>28868</v>
       </c>
       <c r="X8" t="n">
-        <v>44794</v>
+        <v>39376</v>
       </c>
       <c r="Y8" t="n">
-        <v>30015</v>
+        <v>24225</v>
       </c>
       <c r="Z8" t="n">
-        <v>56985</v>
+        <v>56984</v>
       </c>
       <c r="AA8" t="n">
-        <v>62109</v>
+        <v>62107</v>
       </c>
       <c r="AB8" t="n">
-        <v>55208</v>
+        <v>55207</v>
       </c>
       <c r="AC8" t="n">
-        <v>52997</v>
+        <v>52712</v>
       </c>
       <c r="AD8" t="n">
-        <v>86110</v>
+        <v>66279</v>
       </c>
     </row>
     <row r="9">
@@ -1245,91 +1245,91 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>23414</v>
+        <v>16992</v>
       </c>
       <c r="C9" t="n">
-        <v>27158</v>
+        <v>27159</v>
       </c>
       <c r="D9" t="n">
-        <v>130640</v>
+        <v>125774</v>
       </c>
       <c r="E9" t="n">
-        <v>53480</v>
+        <v>43598</v>
       </c>
       <c r="F9" t="n">
-        <v>18255</v>
+        <v>17633</v>
       </c>
       <c r="G9" t="n">
-        <v>31739</v>
+        <v>31738</v>
       </c>
       <c r="H9" t="n">
-        <v>46375</v>
+        <v>46233</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>25212</v>
+        <v>25214</v>
       </c>
       <c r="K9" t="n">
-        <v>25263</v>
+        <v>22407</v>
       </c>
       <c r="L9" t="n">
-        <v>12513</v>
+        <v>12511</v>
       </c>
       <c r="M9" t="n">
-        <v>45687</v>
+        <v>41991</v>
       </c>
       <c r="N9" t="n">
-        <v>55480</v>
+        <v>55392</v>
       </c>
       <c r="O9" t="n">
-        <v>14746</v>
+        <v>14745</v>
       </c>
       <c r="P9" t="n">
-        <v>23961</v>
+        <v>23960</v>
       </c>
       <c r="Q9" t="n">
-        <v>94297</v>
+        <v>94298</v>
       </c>
       <c r="R9" t="n">
-        <v>9022</v>
+        <v>9023</v>
       </c>
       <c r="S9" t="n">
-        <v>16037</v>
+        <v>15223</v>
       </c>
       <c r="T9" t="n">
-        <v>7510</v>
+        <v>7509</v>
       </c>
       <c r="U9" t="n">
-        <v>7589</v>
+        <v>7258</v>
       </c>
       <c r="V9" t="n">
-        <v>68190</v>
+        <v>61996</v>
       </c>
       <c r="W9" t="n">
         <v>26557</v>
       </c>
       <c r="X9" t="n">
-        <v>82154</v>
+        <v>82153</v>
       </c>
       <c r="Y9" t="n">
-        <v>67375</v>
+        <v>67376</v>
       </c>
       <c r="Z9" t="n">
-        <v>15520</v>
+        <v>12285</v>
       </c>
       <c r="AA9" t="n">
-        <v>20643</v>
+        <v>17252</v>
       </c>
       <c r="AB9" t="n">
-        <v>13742</v>
+        <v>11000</v>
       </c>
       <c r="AC9" t="n">
-        <v>8092</v>
+        <v>8079</v>
       </c>
       <c r="AD9" t="n">
-        <v>44644</v>
+        <v>42238</v>
       </c>
     </row>
     <row r="10">
@@ -1339,91 +1339,91 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>22555</v>
+        <v>19992</v>
       </c>
       <c r="C10" t="n">
         <v>28039</v>
       </c>
       <c r="D10" t="n">
-        <v>151943</v>
+        <v>145665</v>
       </c>
       <c r="E10" t="n">
-        <v>44346</v>
+        <v>43187</v>
       </c>
       <c r="F10" t="n">
-        <v>28504</v>
+        <v>24124</v>
       </c>
       <c r="G10" t="n">
-        <v>53042</v>
+        <v>49191</v>
       </c>
       <c r="H10" t="n">
-        <v>67678</v>
+        <v>63828</v>
       </c>
       <c r="I10" t="n">
-        <v>25401</v>
+        <v>25398</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>26747</v>
+        <v>25960</v>
       </c>
       <c r="L10" t="n">
-        <v>41018</v>
+        <v>34095</v>
       </c>
       <c r="M10" t="n">
-        <v>46773</v>
+        <v>44878</v>
       </c>
       <c r="N10" t="n">
-        <v>84949</v>
+        <v>77223</v>
       </c>
       <c r="O10" t="n">
-        <v>36867</v>
+        <v>33343</v>
       </c>
       <c r="P10" t="n">
-        <v>42059</v>
+        <v>39799</v>
       </c>
       <c r="Q10" t="n">
-        <v>115600</v>
+        <v>115599</v>
       </c>
       <c r="R10" t="n">
-        <v>29459</v>
+        <v>27813</v>
       </c>
       <c r="S10" t="n">
-        <v>32838</v>
+        <v>30578</v>
       </c>
       <c r="T10" t="n">
-        <v>31598</v>
+        <v>26802</v>
       </c>
       <c r="U10" t="n">
-        <v>19658</v>
+        <v>19656</v>
       </c>
       <c r="V10" t="n">
         <v>39959</v>
       </c>
       <c r="W10" t="n">
-        <v>49101</v>
+        <v>48388</v>
       </c>
       <c r="X10" t="n">
-        <v>103458</v>
+        <v>102418</v>
       </c>
       <c r="Y10" t="n">
-        <v>88678</v>
+        <v>87267</v>
       </c>
       <c r="Z10" t="n">
-        <v>21731</v>
+        <v>18199</v>
       </c>
       <c r="AA10" t="n">
-        <v>8250</v>
+        <v>7998</v>
       </c>
       <c r="AB10" t="n">
-        <v>19954</v>
+        <v>17167</v>
       </c>
       <c r="AC10" t="n">
-        <v>30629</v>
+        <v>25831</v>
       </c>
       <c r="AD10" t="n">
-        <v>23744</v>
+        <v>20571</v>
       </c>
     </row>
     <row r="11">
@@ -1433,91 +1433,91 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6764</v>
+        <v>6765</v>
       </c>
       <c r="C11" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D11" t="n">
-        <v>150813</v>
+        <v>145947</v>
       </c>
       <c r="E11" t="n">
-        <v>25633</v>
+        <v>25634</v>
       </c>
       <c r="F11" t="n">
-        <v>12757</v>
+        <v>12253</v>
       </c>
       <c r="G11" t="n">
-        <v>51912</v>
+        <v>51911</v>
       </c>
       <c r="H11" t="n">
         <v>66548</v>
       </c>
       <c r="I11" t="n">
-        <v>24270</v>
+        <v>21956</v>
       </c>
       <c r="J11" t="n">
-        <v>26868</v>
+        <v>24427</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>30364</v>
+        <v>27615</v>
       </c>
       <c r="M11" t="n">
-        <v>20614</v>
+        <v>19584</v>
       </c>
       <c r="N11" t="n">
-        <v>74295</v>
+        <v>70763</v>
       </c>
       <c r="O11" t="n">
-        <v>26213</v>
+        <v>24778</v>
       </c>
       <c r="P11" t="n">
-        <v>24753</v>
+        <v>24751</v>
       </c>
       <c r="Q11" t="n">
-        <v>114470</v>
+        <v>114471</v>
       </c>
       <c r="R11" t="n">
-        <v>28328</v>
+        <v>28329</v>
       </c>
       <c r="S11" t="n">
-        <v>22184</v>
+        <v>19584</v>
       </c>
       <c r="T11" t="n">
-        <v>20944</v>
+        <v>20424</v>
       </c>
       <c r="U11" t="n">
-        <v>20230</v>
+        <v>18539</v>
       </c>
       <c r="V11" t="n">
         <v>61062</v>
       </c>
       <c r="W11" t="n">
-        <v>47971</v>
+        <v>45145</v>
       </c>
       <c r="X11" t="n">
-        <v>102327</v>
+        <v>102326</v>
       </c>
       <c r="Y11" t="n">
-        <v>87548</v>
+        <v>87549</v>
       </c>
       <c r="Z11" t="n">
         <v>11670</v>
       </c>
       <c r="AA11" t="n">
-        <v>18259</v>
+        <v>17476</v>
       </c>
       <c r="AB11" t="n">
         <v>13172</v>
       </c>
       <c r="AC11" t="n">
-        <v>19974</v>
+        <v>19453</v>
       </c>
       <c r="AD11" t="n">
-        <v>46169</v>
+        <v>43726</v>
       </c>
     </row>
     <row r="12">
@@ -1527,40 +1527,40 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>29486</v>
+        <v>24161</v>
       </c>
       <c r="C12" t="n">
-        <v>36790</v>
+        <v>34399</v>
       </c>
       <c r="D12" t="n">
-        <v>134592</v>
+        <v>126287</v>
       </c>
       <c r="E12" t="n">
-        <v>59062</v>
+        <v>50931</v>
       </c>
       <c r="F12" t="n">
-        <v>25029</v>
+        <v>21159</v>
       </c>
       <c r="G12" t="n">
-        <v>35692</v>
+        <v>34941</v>
       </c>
       <c r="H12" t="n">
-        <v>50328</v>
+        <v>49064</v>
       </c>
       <c r="I12" t="n">
-        <v>11768</v>
+        <v>11767</v>
       </c>
       <c r="J12" t="n">
-        <v>40656</v>
+        <v>33797</v>
       </c>
       <c r="K12" t="n">
-        <v>31335</v>
+        <v>28310</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>51759</v>
+        <v>44686</v>
       </c>
       <c r="N12" t="n">
         <v>43886</v>
@@ -1569,13 +1569,13 @@
         <v>7859</v>
       </c>
       <c r="P12" t="n">
-        <v>20126</v>
+        <v>18022</v>
       </c>
       <c r="Q12" t="n">
-        <v>98250</v>
+        <v>91119</v>
       </c>
       <c r="R12" t="n">
-        <v>14440</v>
+        <v>14443</v>
       </c>
       <c r="S12" t="n">
         <v>12202</v>
@@ -1584,34 +1584,34 @@
         <v>7128</v>
       </c>
       <c r="U12" t="n">
-        <v>19461</v>
+        <v>19025</v>
       </c>
       <c r="V12" t="n">
-        <v>83634</v>
+        <v>71063</v>
       </c>
       <c r="W12" t="n">
-        <v>19148</v>
+        <v>19149</v>
       </c>
       <c r="X12" t="n">
-        <v>86107</v>
+        <v>80952</v>
       </c>
       <c r="Y12" t="n">
-        <v>71328</v>
+        <v>67889</v>
       </c>
       <c r="Z12" t="n">
-        <v>21882</v>
+        <v>18182</v>
       </c>
       <c r="AA12" t="n">
-        <v>36087</v>
+        <v>26319</v>
       </c>
       <c r="AB12" t="n">
-        <v>16820</v>
+        <v>16540</v>
       </c>
       <c r="AC12" t="n">
         <v>9072</v>
       </c>
       <c r="AD12" t="n">
-        <v>60088</v>
+        <v>51929</v>
       </c>
     </row>
     <row r="13">
@@ -1621,91 +1621,91 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>28940</v>
+        <v>24572</v>
       </c>
       <c r="C13" t="n">
-        <v>64043</v>
+        <v>63609</v>
       </c>
       <c r="D13" t="n">
-        <v>170795</v>
+        <v>165494</v>
       </c>
       <c r="E13" t="n">
         <v>22126</v>
       </c>
       <c r="F13" t="n">
-        <v>32740</v>
+        <v>27033</v>
       </c>
       <c r="G13" t="n">
-        <v>71895</v>
+        <v>71458</v>
       </c>
       <c r="H13" t="n">
-        <v>86531</v>
+        <v>86095</v>
       </c>
       <c r="I13" t="n">
-        <v>44253</v>
+        <v>41503</v>
       </c>
       <c r="J13" t="n">
-        <v>46712</v>
+        <v>43974</v>
       </c>
       <c r="K13" t="n">
-        <v>20637</v>
+        <v>19547</v>
       </c>
       <c r="L13" t="n">
-        <v>50347</v>
+        <v>44694</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>94278</v>
+        <v>81305</v>
       </c>
       <c r="O13" t="n">
-        <v>46196</v>
+        <v>38977</v>
       </c>
       <c r="P13" t="n">
-        <v>35294</v>
+        <v>35293</v>
       </c>
       <c r="Q13" t="n">
-        <v>134453</v>
+        <v>128538</v>
       </c>
       <c r="R13" t="n">
-        <v>48311</v>
+        <v>47876</v>
       </c>
       <c r="S13" t="n">
-        <v>42167</v>
+        <v>33783</v>
       </c>
       <c r="T13" t="n">
-        <v>40927</v>
+        <v>39971</v>
       </c>
       <c r="U13" t="n">
-        <v>40212</v>
+        <v>38086</v>
       </c>
       <c r="V13" t="n">
-        <v>76015</v>
+        <v>75963</v>
       </c>
       <c r="W13" t="n">
-        <v>67954</v>
+        <v>63843</v>
       </c>
       <c r="X13" t="n">
-        <v>122310</v>
+        <v>121409</v>
       </c>
       <c r="Y13" t="n">
-        <v>107531</v>
+        <v>107096</v>
       </c>
       <c r="Z13" t="n">
-        <v>31653</v>
+        <v>30793</v>
       </c>
       <c r="AA13" t="n">
-        <v>38104</v>
+        <v>36859</v>
       </c>
       <c r="AB13" t="n">
-        <v>33155</v>
+        <v>32295</v>
       </c>
       <c r="AC13" t="n">
-        <v>39957</v>
+        <v>39000</v>
       </c>
       <c r="AD13" t="n">
-        <v>66014</v>
+        <v>63273</v>
       </c>
     </row>
     <row r="14">
@@ -1715,91 +1715,91 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>72650</v>
+        <v>67584</v>
       </c>
       <c r="C14" t="n">
-        <v>64303</v>
+        <v>62517</v>
       </c>
       <c r="D14" t="n">
         <v>86417</v>
       </c>
       <c r="E14" t="n">
-        <v>102226</v>
+        <v>94276</v>
       </c>
       <c r="F14" t="n">
-        <v>68193</v>
+        <v>64504</v>
       </c>
       <c r="G14" t="n">
-        <v>39824</v>
+        <v>39825</v>
       </c>
       <c r="H14" t="n">
-        <v>37529</v>
+        <v>37528</v>
       </c>
       <c r="I14" t="n">
-        <v>55021</v>
+        <v>55024</v>
       </c>
       <c r="J14" t="n">
-        <v>83820</v>
+        <v>77039</v>
       </c>
       <c r="K14" t="n">
-        <v>74499</v>
+        <v>69602</v>
       </c>
       <c r="L14" t="n">
         <v>43434</v>
       </c>
       <c r="M14" t="n">
-        <v>94923</v>
+        <v>81579</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>51612</v>
+        <v>51293</v>
       </c>
       <c r="P14" t="n">
         <v>46209</v>
       </c>
       <c r="Q14" t="n">
-        <v>47231</v>
+        <v>47233</v>
       </c>
       <c r="R14" t="n">
-        <v>61755</v>
+        <v>50173</v>
       </c>
       <c r="S14" t="n">
-        <v>56479</v>
+        <v>55636</v>
       </c>
       <c r="T14" t="n">
         <v>50473</v>
       </c>
       <c r="U14" t="n">
-        <v>71006</v>
+        <v>59425</v>
       </c>
       <c r="V14" t="n">
-        <v>126797</v>
+        <v>114408</v>
       </c>
       <c r="W14" t="n">
-        <v>28774</v>
+        <v>28775</v>
       </c>
       <c r="X14" t="n">
-        <v>40103</v>
+        <v>40104</v>
       </c>
       <c r="Y14" t="n">
-        <v>54550</v>
+        <v>47044</v>
       </c>
       <c r="Z14" t="n">
-        <v>65046</v>
+        <v>61527</v>
       </c>
       <c r="AA14" t="n">
-        <v>79251</v>
+        <v>69664</v>
       </c>
       <c r="AB14" t="n">
-        <v>65968</v>
+        <v>59885</v>
       </c>
       <c r="AC14" t="n">
-        <v>63194</v>
+        <v>52417</v>
       </c>
       <c r="AD14" t="n">
-        <v>103252</v>
+        <v>88342</v>
       </c>
     </row>
     <row r="15">
@@ -1809,91 +1809,91 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>23734</v>
+        <v>21512</v>
       </c>
       <c r="C15" t="n">
-        <v>48074</v>
+        <v>41357</v>
       </c>
       <c r="D15" t="n">
-        <v>154826</v>
+        <v>132151</v>
       </c>
       <c r="E15" t="n">
-        <v>53310</v>
+        <v>48248</v>
       </c>
       <c r="F15" t="n">
-        <v>19277</v>
+        <v>17262</v>
       </c>
       <c r="G15" t="n">
-        <v>55925</v>
+        <v>42293</v>
       </c>
       <c r="H15" t="n">
-        <v>70561</v>
+        <v>54928</v>
       </c>
       <c r="I15" t="n">
         <v>14198</v>
       </c>
       <c r="J15" t="n">
-        <v>34904</v>
+        <v>34310</v>
       </c>
       <c r="K15" t="n">
-        <v>25583</v>
+        <v>25541</v>
       </c>
       <c r="L15" t="n">
-        <v>7983</v>
+        <v>7984</v>
       </c>
       <c r="M15" t="n">
-        <v>46007</v>
+        <v>39096</v>
       </c>
       <c r="N15" t="n">
-        <v>50172</v>
+        <v>48930</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>12070</v>
+        <v>10163</v>
       </c>
       <c r="Q15" t="n">
-        <v>118483</v>
+        <v>96163</v>
       </c>
       <c r="R15" t="n">
-        <v>32341</v>
+        <v>21795</v>
       </c>
       <c r="S15" t="n">
-        <v>5650</v>
+        <v>5649</v>
       </c>
       <c r="T15" t="n">
-        <v>9234</v>
+        <v>8869</v>
       </c>
       <c r="U15" t="n">
-        <v>24243</v>
+        <v>20119</v>
       </c>
       <c r="V15" t="n">
-        <v>77881</v>
+        <v>71576</v>
       </c>
       <c r="W15" t="n">
         <v>26129</v>
       </c>
       <c r="X15" t="n">
-        <v>106340</v>
+        <v>88778</v>
       </c>
       <c r="Y15" t="n">
-        <v>91561</v>
+        <v>73753</v>
       </c>
       <c r="Z15" t="n">
-        <v>16130</v>
+        <v>16131</v>
       </c>
       <c r="AA15" t="n">
-        <v>30335</v>
+        <v>26832</v>
       </c>
       <c r="AB15" t="n">
-        <v>17052</v>
+        <v>17053</v>
       </c>
       <c r="AC15" t="n">
         <v>10583</v>
       </c>
       <c r="AD15" t="n">
-        <v>54336</v>
+        <v>53609</v>
       </c>
     </row>
     <row r="16">
@@ -1903,82 +1903,82 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>30884</v>
+        <v>29823</v>
       </c>
       <c r="C16" t="n">
-        <v>55224</v>
+        <v>50008</v>
       </c>
       <c r="D16" t="n">
-        <v>161976</v>
+        <v>132893</v>
       </c>
       <c r="E16" t="n">
-        <v>60460</v>
+        <v>49347</v>
       </c>
       <c r="F16" t="n">
-        <v>20820</v>
+        <v>20822</v>
       </c>
       <c r="G16" t="n">
-        <v>63075</v>
+        <v>52146</v>
       </c>
       <c r="H16" t="n">
-        <v>77711</v>
+        <v>64445</v>
       </c>
       <c r="I16" t="n">
         <v>22849</v>
       </c>
       <c r="J16" t="n">
-        <v>42054</v>
+        <v>41459</v>
       </c>
       <c r="K16" t="n">
         <v>23713</v>
       </c>
       <c r="L16" t="n">
-        <v>19365</v>
+        <v>18644</v>
       </c>
       <c r="M16" t="n">
-        <v>35730</v>
+        <v>35729</v>
       </c>
       <c r="N16" t="n">
-        <v>46478</v>
+        <v>46476</v>
       </c>
       <c r="O16" t="n">
-        <v>11854</v>
+        <v>10660</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>125633</v>
+        <v>93709</v>
       </c>
       <c r="R16" t="n">
-        <v>39491</v>
+        <v>31031</v>
       </c>
       <c r="S16" t="n">
-        <v>11001</v>
+        <v>11002</v>
       </c>
       <c r="T16" t="n">
-        <v>17479</v>
+        <v>17480</v>
       </c>
       <c r="U16" t="n">
-        <v>31393</v>
+        <v>28365</v>
       </c>
       <c r="V16" t="n">
-        <v>85031</v>
+        <v>78725</v>
       </c>
       <c r="W16" t="n">
-        <v>35645</v>
+        <v>35646</v>
       </c>
       <c r="X16" t="n">
-        <v>113490</v>
+        <v>86580</v>
       </c>
       <c r="Y16" t="n">
-        <v>98711</v>
+        <v>83270</v>
       </c>
       <c r="Z16" t="n">
         <v>23280</v>
       </c>
       <c r="AA16" t="n">
-        <v>37485</v>
+        <v>33981</v>
       </c>
       <c r="AB16" t="n">
         <v>24202</v>
@@ -1987,7 +1987,7 @@
         <v>19176</v>
       </c>
       <c r="AD16" t="n">
-        <v>61485</v>
+        <v>60758</v>
       </c>
     </row>
     <row r="17">
@@ -1997,91 +1997,91 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>113166</v>
+        <v>110779</v>
       </c>
       <c r="C17" t="n">
-        <v>90647</v>
+        <v>90648</v>
       </c>
       <c r="D17" t="n">
         <v>39670</v>
       </c>
       <c r="E17" t="n">
-        <v>143232</v>
+        <v>137385</v>
       </c>
       <c r="F17" t="n">
-        <v>112045</v>
+        <v>111234</v>
       </c>
       <c r="G17" t="n">
-        <v>66501</v>
+        <v>66503</v>
       </c>
       <c r="H17" t="n">
-        <v>56657</v>
+        <v>53193</v>
       </c>
       <c r="I17" t="n">
-        <v>94594</v>
+        <v>94595</v>
       </c>
       <c r="J17" t="n">
-        <v>114965</v>
+        <v>114425</v>
       </c>
       <c r="K17" t="n">
         <v>115015</v>
       </c>
       <c r="L17" t="n">
-        <v>98164</v>
+        <v>90666</v>
       </c>
       <c r="M17" t="n">
-        <v>135439</v>
+        <v>128811</v>
       </c>
       <c r="N17" t="n">
-        <v>47230</v>
+        <v>47232</v>
       </c>
       <c r="O17" t="n">
-        <v>120408</v>
+        <v>98525</v>
       </c>
       <c r="P17" t="n">
-        <v>125600</v>
+        <v>93441</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>88099</v>
+        <v>88100</v>
       </c>
       <c r="S17" t="n">
-        <v>116379</v>
+        <v>102868</v>
       </c>
       <c r="T17" t="n">
-        <v>99340</v>
+        <v>97705</v>
       </c>
       <c r="U17" t="n">
-        <v>97350</v>
+        <v>97352</v>
       </c>
       <c r="V17" t="n">
-        <v>157943</v>
+        <v>143979</v>
       </c>
       <c r="W17" t="n">
-        <v>80264</v>
+        <v>75447</v>
       </c>
       <c r="X17" t="n">
         <v>15392</v>
       </c>
       <c r="Y17" t="n">
-        <v>41323</v>
+        <v>37024</v>
       </c>
       <c r="Z17" t="n">
         <v>105272</v>
       </c>
       <c r="AA17" t="n">
-        <v>110396</v>
+        <v>110395</v>
       </c>
       <c r="AB17" t="n">
         <v>103495</v>
       </c>
       <c r="AC17" t="n">
-        <v>101284</v>
+        <v>99649</v>
       </c>
       <c r="AD17" t="n">
-        <v>134397</v>
+        <v>116473</v>
       </c>
     </row>
     <row r="18">
@@ -2091,91 +2091,91 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>29059</v>
+        <v>23257</v>
       </c>
       <c r="C18" t="n">
-        <v>28243</v>
+        <v>22493</v>
       </c>
       <c r="D18" t="n">
-        <v>124893</v>
+        <v>120027</v>
       </c>
       <c r="E18" t="n">
-        <v>59125</v>
+        <v>49863</v>
       </c>
       <c r="F18" t="n">
-        <v>27938</v>
+        <v>24659</v>
       </c>
       <c r="G18" t="n">
-        <v>25992</v>
+        <v>25991</v>
       </c>
       <c r="H18" t="n">
-        <v>40628</v>
+        <v>40627</v>
       </c>
       <c r="I18" t="n">
-        <v>9166</v>
+        <v>9167</v>
       </c>
       <c r="J18" t="n">
-        <v>30858</v>
+        <v>28039</v>
       </c>
       <c r="K18" t="n">
-        <v>30908</v>
+        <v>28672</v>
       </c>
       <c r="L18" t="n">
-        <v>13851</v>
+        <v>13852</v>
       </c>
       <c r="M18" t="n">
-        <v>51332</v>
+        <v>48256</v>
       </c>
       <c r="N18" t="n">
-        <v>61693</v>
+        <v>50886</v>
       </c>
       <c r="O18" t="n">
-        <v>36301</v>
+        <v>21629</v>
       </c>
       <c r="P18" t="n">
-        <v>41493</v>
+        <v>31599</v>
       </c>
       <c r="Q18" t="n">
-        <v>88550</v>
+        <v>88551</v>
       </c>
       <c r="R18" t="n">
         <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>32272</v>
+        <v>23553</v>
       </c>
       <c r="T18" t="n">
-        <v>15147</v>
+        <v>15026</v>
       </c>
       <c r="U18" t="n">
-        <v>13243</v>
+        <v>10916</v>
       </c>
       <c r="V18" t="n">
-        <v>73836</v>
+        <v>66521</v>
       </c>
       <c r="W18" t="n">
         <v>22051</v>
       </c>
       <c r="X18" t="n">
-        <v>76407</v>
+        <v>76406</v>
       </c>
       <c r="Y18" t="n">
-        <v>61628</v>
+        <v>61629</v>
       </c>
       <c r="Z18" t="n">
-        <v>21165</v>
+        <v>18697</v>
       </c>
       <c r="AA18" t="n">
-        <v>26289</v>
+        <v>23517</v>
       </c>
       <c r="AB18" t="n">
-        <v>19388</v>
+        <v>17665</v>
       </c>
       <c r="AC18" t="n">
-        <v>17091</v>
+        <v>16005</v>
       </c>
       <c r="AD18" t="n">
-        <v>50290</v>
+        <v>43383</v>
       </c>
     </row>
     <row r="19">
@@ -2185,91 +2185,91 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>21043</v>
+        <v>18821</v>
       </c>
       <c r="C19" t="n">
-        <v>45383</v>
+        <v>41822</v>
       </c>
       <c r="D19" t="n">
-        <v>152135</v>
+        <v>137455</v>
       </c>
       <c r="E19" t="n">
-        <v>50619</v>
+        <v>45557</v>
       </c>
       <c r="F19" t="n">
-        <v>12394</v>
+        <v>12395</v>
       </c>
       <c r="G19" t="n">
-        <v>53234</v>
+        <v>43960</v>
       </c>
       <c r="H19" t="n">
-        <v>67870</v>
+        <v>58455</v>
       </c>
       <c r="I19" t="n">
         <v>14663</v>
       </c>
       <c r="J19" t="n">
-        <v>32213</v>
+        <v>31619</v>
       </c>
       <c r="K19" t="n">
-        <v>22892</v>
+        <v>20635</v>
       </c>
       <c r="L19" t="n">
-        <v>12381</v>
+        <v>12335</v>
       </c>
       <c r="M19" t="n">
-        <v>43316</v>
+        <v>34229</v>
       </c>
       <c r="N19" t="n">
-        <v>56312</v>
+        <v>54234</v>
       </c>
       <c r="O19" t="n">
-        <v>5977</v>
+        <v>5976</v>
       </c>
       <c r="P19" t="n">
         <v>10739</v>
       </c>
       <c r="Q19" t="n">
-        <v>115792</v>
+        <v>101467</v>
       </c>
       <c r="R19" t="n">
-        <v>29650</v>
+        <v>22711</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>9293</v>
+        <v>9294</v>
       </c>
       <c r="U19" t="n">
-        <v>21552</v>
+        <v>19117</v>
       </c>
       <c r="V19" t="n">
-        <v>75190</v>
+        <v>68070</v>
       </c>
       <c r="W19" t="n">
-        <v>32416</v>
+        <v>30852</v>
       </c>
       <c r="X19" t="n">
-        <v>103649</v>
+        <v>93287</v>
       </c>
       <c r="Y19" t="n">
-        <v>88870</v>
+        <v>79057</v>
       </c>
       <c r="Z19" t="n">
-        <v>13439</v>
+        <v>13142</v>
       </c>
       <c r="AA19" t="n">
-        <v>27644</v>
+        <v>23393</v>
       </c>
       <c r="AB19" t="n">
-        <v>14361</v>
+        <v>14362</v>
       </c>
       <c r="AC19" t="n">
-        <v>10990</v>
+        <v>10127</v>
       </c>
       <c r="AD19" t="n">
-        <v>51645</v>
+        <v>50918</v>
       </c>
     </row>
     <row r="20">
@@ -2279,55 +2279,55 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>19451</v>
+        <v>17229</v>
       </c>
       <c r="C20" t="n">
-        <v>34578</v>
+        <v>34184</v>
       </c>
       <c r="D20" t="n">
-        <v>135224</v>
+        <v>130358</v>
       </c>
       <c r="E20" t="n">
-        <v>49027</v>
+        <v>43921</v>
       </c>
       <c r="F20" t="n">
-        <v>14993</v>
+        <v>14149</v>
       </c>
       <c r="G20" t="n">
-        <v>36323</v>
+        <v>36322</v>
       </c>
       <c r="H20" t="n">
-        <v>50959</v>
+        <v>50817</v>
       </c>
       <c r="I20" t="n">
-        <v>7026</v>
+        <v>7025</v>
       </c>
       <c r="J20" t="n">
-        <v>30620</v>
+        <v>26787</v>
       </c>
       <c r="K20" t="n">
         <v>21300</v>
       </c>
       <c r="L20" t="n">
-        <v>7310</v>
+        <v>7309</v>
       </c>
       <c r="M20" t="n">
-        <v>41724</v>
+        <v>39256</v>
       </c>
       <c r="N20" t="n">
-        <v>50566</v>
+        <v>50563</v>
       </c>
       <c r="O20" t="n">
-        <v>9543</v>
+        <v>9297</v>
       </c>
       <c r="P20" t="n">
-        <v>17230</v>
+        <v>17229</v>
       </c>
       <c r="Q20" t="n">
-        <v>98881</v>
+        <v>97796</v>
       </c>
       <c r="R20" t="n">
-        <v>15206</v>
+        <v>15073</v>
       </c>
       <c r="S20" t="n">
         <v>9305</v>
@@ -2336,34 +2336,34 @@
         <v>0</v>
       </c>
       <c r="U20" t="n">
-        <v>12349</v>
+        <v>12351</v>
       </c>
       <c r="V20" t="n">
-        <v>73598</v>
+        <v>64053</v>
       </c>
       <c r="W20" t="n">
         <v>25397</v>
       </c>
       <c r="X20" t="n">
-        <v>86739</v>
+        <v>86737</v>
       </c>
       <c r="Y20" t="n">
-        <v>71959</v>
+        <v>71960</v>
       </c>
       <c r="Z20" t="n">
-        <v>11847</v>
+        <v>11172</v>
       </c>
       <c r="AA20" t="n">
-        <v>26051</v>
+        <v>19309</v>
       </c>
       <c r="AB20" t="n">
-        <v>10369</v>
+        <v>9530</v>
       </c>
       <c r="AC20" t="n">
-        <v>2061</v>
+        <v>2062</v>
       </c>
       <c r="AD20" t="n">
-        <v>50052</v>
+        <v>46086</v>
       </c>
     </row>
     <row r="21">
@@ -2373,91 +2373,91 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>18173</v>
+        <v>13427</v>
       </c>
       <c r="C21" t="n">
-        <v>27618</v>
+        <v>27619</v>
       </c>
       <c r="D21" t="n">
-        <v>134370</v>
+        <v>129504</v>
       </c>
       <c r="E21" t="n">
-        <v>48239</v>
+        <v>40033</v>
       </c>
       <c r="F21" t="n">
-        <v>17052</v>
+        <v>14829</v>
       </c>
       <c r="G21" t="n">
-        <v>35469</v>
+        <v>35468</v>
       </c>
       <c r="H21" t="n">
         <v>50105</v>
       </c>
       <c r="I21" t="n">
-        <v>7389</v>
+        <v>7116</v>
       </c>
       <c r="J21" t="n">
-        <v>19972</v>
+        <v>19973</v>
       </c>
       <c r="K21" t="n">
-        <v>20022</v>
+        <v>18842</v>
       </c>
       <c r="L21" t="n">
-        <v>18909</v>
+        <v>18628</v>
       </c>
       <c r="M21" t="n">
-        <v>40446</v>
+        <v>38426</v>
       </c>
       <c r="N21" t="n">
-        <v>71170</v>
+        <v>60363</v>
       </c>
       <c r="O21" t="n">
-        <v>25415</v>
+        <v>20434</v>
       </c>
       <c r="P21" t="n">
-        <v>30607</v>
+        <v>28029</v>
       </c>
       <c r="Q21" t="n">
-        <v>98027</v>
+        <v>98028</v>
       </c>
       <c r="R21" t="n">
         <v>10988</v>
       </c>
       <c r="S21" t="n">
-        <v>21386</v>
+        <v>18947</v>
       </c>
       <c r="T21" t="n">
-        <v>12230</v>
+        <v>12229</v>
       </c>
       <c r="U21" t="n">
         <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>62950</v>
+        <v>58431</v>
       </c>
       <c r="W21" t="n">
         <v>31528</v>
       </c>
       <c r="X21" t="n">
-        <v>85884</v>
+        <v>85883</v>
       </c>
       <c r="Y21" t="n">
-        <v>71105</v>
+        <v>71106</v>
       </c>
       <c r="Z21" t="n">
-        <v>10279</v>
+        <v>8867</v>
       </c>
       <c r="AA21" t="n">
-        <v>15403</v>
+        <v>13687</v>
       </c>
       <c r="AB21" t="n">
-        <v>8502</v>
+        <v>7835</v>
       </c>
       <c r="AC21" t="n">
-        <v>11260</v>
+        <v>11258</v>
       </c>
       <c r="AD21" t="n">
-        <v>39404</v>
+        <v>39272</v>
       </c>
     </row>
     <row r="22">
@@ -2467,91 +2467,91 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>62328</v>
+        <v>55637</v>
       </c>
       <c r="C22" t="n">
-        <v>53700</v>
+        <v>53701</v>
       </c>
       <c r="D22" t="n">
-        <v>194809</v>
+        <v>175464</v>
       </c>
       <c r="E22" t="n">
-        <v>62570</v>
+        <v>58479</v>
       </c>
       <c r="F22" t="n">
-        <v>71370</v>
+        <v>60143</v>
       </c>
       <c r="G22" t="n">
-        <v>95908</v>
+        <v>81154</v>
       </c>
       <c r="H22" t="n">
-        <v>110544</v>
+        <v>95318</v>
       </c>
       <c r="I22" t="n">
-        <v>68266</v>
+        <v>62810</v>
       </c>
       <c r="J22" t="n">
         <v>39963</v>
       </c>
       <c r="K22" t="n">
-        <v>66521</v>
+        <v>61056</v>
       </c>
       <c r="L22" t="n">
-        <v>83884</v>
+        <v>72345</v>
       </c>
       <c r="M22" t="n">
-        <v>75823</v>
+        <v>75770</v>
       </c>
       <c r="N22" t="n">
-        <v>127815</v>
+        <v>115599</v>
       </c>
       <c r="O22" t="n">
-        <v>79733</v>
+        <v>70086</v>
       </c>
       <c r="P22" t="n">
-        <v>84925</v>
+        <v>76542</v>
       </c>
       <c r="Q22" t="n">
-        <v>158466</v>
+        <v>144379</v>
       </c>
       <c r="R22" t="n">
-        <v>72324</v>
+        <v>67776</v>
       </c>
       <c r="S22" t="n">
-        <v>75704</v>
+        <v>67321</v>
       </c>
       <c r="T22" t="n">
-        <v>74464</v>
+        <v>65052</v>
       </c>
       <c r="U22" t="n">
-        <v>62523</v>
+        <v>58121</v>
       </c>
       <c r="V22" t="n">
         <v>0</v>
       </c>
       <c r="W22" t="n">
-        <v>91967</v>
+        <v>88351</v>
       </c>
       <c r="X22" t="n">
-        <v>146323</v>
+        <v>132234</v>
       </c>
       <c r="Y22" t="n">
-        <v>131544</v>
+        <v>117066</v>
       </c>
       <c r="Z22" t="n">
-        <v>64597</v>
+        <v>54942</v>
       </c>
       <c r="AA22" t="n">
-        <v>44968</v>
+        <v>44969</v>
       </c>
       <c r="AB22" t="n">
-        <v>62820</v>
+        <v>55417</v>
       </c>
       <c r="AC22" t="n">
-        <v>73494</v>
+        <v>64081</v>
       </c>
       <c r="AD22" t="n">
-        <v>28386</v>
+        <v>28387</v>
       </c>
     </row>
     <row r="23">
@@ -2561,91 +2561,91 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>47290</v>
+        <v>42567</v>
       </c>
       <c r="C23" t="n">
-        <v>35504</v>
+        <v>35505</v>
       </c>
       <c r="D23" t="n">
-        <v>117768</v>
+        <v>107138</v>
       </c>
       <c r="E23" t="n">
-        <v>77356</v>
+        <v>69337</v>
       </c>
       <c r="F23" t="n">
-        <v>43759</v>
+        <v>39565</v>
       </c>
       <c r="G23" t="n">
-        <v>18780</v>
+        <v>18779</v>
       </c>
       <c r="H23" t="n">
-        <v>33504</v>
+        <v>29915</v>
       </c>
       <c r="I23" t="n">
-        <v>27073</v>
+        <v>27074</v>
       </c>
       <c r="J23" t="n">
-        <v>49088</v>
+        <v>49089</v>
       </c>
       <c r="K23" t="n">
-        <v>49139</v>
+        <v>46716</v>
       </c>
       <c r="L23" t="n">
         <v>18406</v>
       </c>
       <c r="M23" t="n">
-        <v>69563</v>
+        <v>63092</v>
       </c>
       <c r="N23" t="n">
         <v>28835</v>
       </c>
       <c r="O23" t="n">
-        <v>27016</v>
+        <v>26265</v>
       </c>
       <c r="P23" t="n">
         <v>35027</v>
       </c>
       <c r="Q23" t="n">
-        <v>81426</v>
+        <v>76034</v>
       </c>
       <c r="R23" t="n">
         <v>22223</v>
       </c>
       <c r="S23" t="n">
-        <v>32045</v>
+        <v>30608</v>
       </c>
       <c r="T23" t="n">
-        <v>26058</v>
+        <v>25534</v>
       </c>
       <c r="U23" t="n">
-        <v>31474</v>
+        <v>31475</v>
       </c>
       <c r="V23" t="n">
-        <v>92066</v>
+        <v>87818</v>
       </c>
       <c r="W23" t="n">
         <v>0</v>
       </c>
       <c r="X23" t="n">
-        <v>69283</v>
+        <v>63765</v>
       </c>
       <c r="Y23" t="n">
-        <v>54504</v>
+        <v>48740</v>
       </c>
       <c r="Z23" t="n">
-        <v>39396</v>
+        <v>36588</v>
       </c>
       <c r="AA23" t="n">
-        <v>44519</v>
+        <v>44326</v>
       </c>
       <c r="AB23" t="n">
-        <v>37618</v>
+        <v>34946</v>
       </c>
       <c r="AC23" t="n">
-        <v>28002</v>
+        <v>27478</v>
       </c>
       <c r="AD23" t="n">
-        <v>68520</v>
+        <v>61330</v>
       </c>
     </row>
     <row r="24">
@@ -2655,70 +2655,70 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>99484</v>
+        <v>95937</v>
       </c>
       <c r="C24" t="n">
-        <v>76965</v>
+        <v>75444</v>
       </c>
       <c r="D24" t="n">
         <v>47882</v>
       </c>
       <c r="E24" t="n">
-        <v>129550</v>
+        <v>122543</v>
       </c>
       <c r="F24" t="n">
-        <v>98363</v>
+        <v>97011</v>
       </c>
       <c r="G24" t="n">
-        <v>52819</v>
+        <v>51299</v>
       </c>
       <c r="H24" t="n">
-        <v>42975</v>
+        <v>37801</v>
       </c>
       <c r="I24" t="n">
-        <v>80912</v>
+        <v>79391</v>
       </c>
       <c r="J24" t="n">
-        <v>101283</v>
+        <v>99221</v>
       </c>
       <c r="K24" t="n">
-        <v>101333</v>
+        <v>100792</v>
       </c>
       <c r="L24" t="n">
-        <v>84482</v>
+        <v>80038</v>
       </c>
       <c r="M24" t="n">
-        <v>121757</v>
+        <v>120376</v>
       </c>
       <c r="N24" t="n">
-        <v>39796</v>
+        <v>39797</v>
       </c>
       <c r="O24" t="n">
-        <v>106726</v>
+        <v>87897</v>
       </c>
       <c r="P24" t="n">
-        <v>111918</v>
+        <v>86006</v>
       </c>
       <c r="Q24" t="n">
-        <v>16928</v>
+        <v>16074</v>
       </c>
       <c r="R24" t="n">
-        <v>74417</v>
+        <v>72896</v>
       </c>
       <c r="S24" t="n">
-        <v>102697</v>
+        <v>92240</v>
       </c>
       <c r="T24" t="n">
-        <v>85658</v>
+        <v>84136</v>
       </c>
       <c r="U24" t="n">
-        <v>83668</v>
+        <v>82510</v>
       </c>
       <c r="V24" t="n">
-        <v>144260</v>
+        <v>128775</v>
       </c>
       <c r="W24" t="n">
-        <v>66582</v>
+        <v>61632</v>
       </c>
       <c r="X24" t="n">
         <v>0</v>
@@ -2727,19 +2727,19 @@
         <v>21781</v>
       </c>
       <c r="Z24" t="n">
-        <v>91590</v>
+        <v>91049</v>
       </c>
       <c r="AA24" t="n">
-        <v>96714</v>
+        <v>96172</v>
       </c>
       <c r="AB24" t="n">
-        <v>89812</v>
+        <v>89272</v>
       </c>
       <c r="AC24" t="n">
-        <v>87602</v>
+        <v>86080</v>
       </c>
       <c r="AD24" t="n">
-        <v>120715</v>
+        <v>101269</v>
       </c>
     </row>
     <row r="25">
@@ -2749,91 +2749,91 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>85955</v>
+        <v>83566</v>
       </c>
       <c r="C25" t="n">
-        <v>63436</v>
+        <v>63346</v>
       </c>
       <c r="D25" t="n">
-        <v>78077</v>
+        <v>58398</v>
       </c>
       <c r="E25" t="n">
-        <v>116020</v>
+        <v>110172</v>
       </c>
       <c r="F25" t="n">
-        <v>84833</v>
+        <v>84021</v>
       </c>
       <c r="G25" t="n">
-        <v>39289</v>
+        <v>38801</v>
       </c>
       <c r="H25" t="n">
-        <v>29446</v>
+        <v>24254</v>
       </c>
       <c r="I25" t="n">
-        <v>67382</v>
+        <v>67293</v>
       </c>
       <c r="J25" t="n">
-        <v>87753</v>
+        <v>86723</v>
       </c>
       <c r="K25" t="n">
-        <v>87803</v>
+        <v>87802</v>
       </c>
       <c r="L25" t="n">
-        <v>70953</v>
+        <v>66610</v>
       </c>
       <c r="M25" t="n">
-        <v>108227</v>
+        <v>107386</v>
       </c>
       <c r="N25" t="n">
-        <v>53092</v>
+        <v>47090</v>
       </c>
       <c r="O25" t="n">
-        <v>93196</v>
+        <v>74469</v>
       </c>
       <c r="P25" t="n">
-        <v>98389</v>
+        <v>83231</v>
       </c>
       <c r="Q25" t="n">
-        <v>41734</v>
+        <v>37149</v>
       </c>
       <c r="R25" t="n">
-        <v>60888</v>
+        <v>60798</v>
       </c>
       <c r="S25" t="n">
-        <v>89168</v>
+        <v>78812</v>
       </c>
       <c r="T25" t="n">
-        <v>72128</v>
+        <v>72038</v>
       </c>
       <c r="U25" t="n">
         <v>70139</v>
       </c>
       <c r="V25" t="n">
-        <v>130731</v>
+        <v>116677</v>
       </c>
       <c r="W25" t="n">
-        <v>53052</v>
+        <v>48204</v>
       </c>
       <c r="X25" t="n">
-        <v>21500</v>
+        <v>21499</v>
       </c>
       <c r="Y25" t="n">
         <v>0</v>
       </c>
       <c r="Z25" t="n">
-        <v>78060</v>
+        <v>78059</v>
       </c>
       <c r="AA25" t="n">
-        <v>83184</v>
+        <v>83182</v>
       </c>
       <c r="AB25" t="n">
-        <v>76283</v>
+        <v>76282</v>
       </c>
       <c r="AC25" t="n">
-        <v>74072</v>
+        <v>73982</v>
       </c>
       <c r="AD25" t="n">
-        <v>107185</v>
+        <v>89171</v>
       </c>
     </row>
     <row r="26">
@@ -2843,91 +2843,91 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>11101</v>
+        <v>7706</v>
       </c>
       <c r="C26" t="n">
-        <v>35441</v>
+        <v>35443</v>
       </c>
       <c r="D26" t="n">
-        <v>142193</v>
+        <v>137098</v>
       </c>
       <c r="E26" t="n">
-        <v>40677</v>
+        <v>35157</v>
       </c>
       <c r="F26" t="n">
-        <v>5963</v>
+        <v>5962</v>
       </c>
       <c r="G26" t="n">
-        <v>43292</v>
+        <v>43062</v>
       </c>
       <c r="H26" t="n">
-        <v>57928</v>
+        <v>57557</v>
       </c>
       <c r="I26" t="n">
-        <v>13643</v>
+        <v>11324</v>
       </c>
       <c r="J26" t="n">
-        <v>22271</v>
+        <v>18520</v>
       </c>
       <c r="K26" t="n">
-        <v>12950</v>
+        <v>12754</v>
       </c>
       <c r="L26" t="n">
-        <v>20558</v>
+        <v>17575</v>
       </c>
       <c r="M26" t="n">
-        <v>33374</v>
+        <v>31946</v>
       </c>
       <c r="N26" t="n">
-        <v>64489</v>
+        <v>60931</v>
       </c>
       <c r="O26" t="n">
-        <v>16407</v>
+        <v>15144</v>
       </c>
       <c r="P26" t="n">
         <v>21600</v>
       </c>
       <c r="Q26" t="n">
-        <v>105850</v>
+        <v>105622</v>
       </c>
       <c r="R26" t="n">
-        <v>19708</v>
+        <v>19014</v>
       </c>
       <c r="S26" t="n">
-        <v>12378</v>
+        <v>12379</v>
       </c>
       <c r="T26" t="n">
-        <v>11138</v>
+        <v>10384</v>
       </c>
       <c r="U26" t="n">
-        <v>11610</v>
+        <v>9086</v>
       </c>
       <c r="V26" t="n">
-        <v>65249</v>
+        <v>55786</v>
       </c>
       <c r="W26" t="n">
-        <v>39351</v>
+        <v>34885</v>
       </c>
       <c r="X26" t="n">
-        <v>93708</v>
+        <v>93477</v>
       </c>
       <c r="Y26" t="n">
-        <v>78928</v>
+        <v>78700</v>
       </c>
       <c r="Z26" t="n">
         <v>0</v>
       </c>
       <c r="AA26" t="n">
-        <v>17702</v>
+        <v>11042</v>
       </c>
       <c r="AB26" t="n">
-        <v>2499</v>
+        <v>2500</v>
       </c>
       <c r="AC26" t="n">
-        <v>10169</v>
+        <v>9413</v>
       </c>
       <c r="AD26" t="n">
-        <v>41703</v>
+        <v>37819</v>
       </c>
     </row>
     <row r="27">
@@ -2937,91 +2937,91 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>14125</v>
+        <v>12783</v>
       </c>
       <c r="C27" t="n">
-        <v>39488</v>
+        <v>33850</v>
       </c>
       <c r="D27" t="n">
-        <v>146240</v>
+        <v>141374</v>
       </c>
       <c r="E27" t="n">
-        <v>35916</v>
+        <v>35189</v>
       </c>
       <c r="F27" t="n">
-        <v>22858</v>
+        <v>17601</v>
       </c>
       <c r="G27" t="n">
-        <v>47340</v>
+        <v>47338</v>
       </c>
       <c r="H27" t="n">
-        <v>61976</v>
+        <v>61975</v>
       </c>
       <c r="I27" t="n">
-        <v>19698</v>
+        <v>18037</v>
       </c>
       <c r="J27" t="n">
         <v>8276</v>
       </c>
       <c r="K27" t="n">
-        <v>18318</v>
+        <v>18319</v>
       </c>
       <c r="L27" t="n">
-        <v>35315</v>
+        <v>27572</v>
       </c>
       <c r="M27" t="n">
-        <v>38344</v>
+        <v>37903</v>
       </c>
       <c r="N27" t="n">
-        <v>79247</v>
+        <v>70826</v>
       </c>
       <c r="O27" t="n">
-        <v>31165</v>
+        <v>26820</v>
       </c>
       <c r="P27" t="n">
-        <v>36357</v>
+        <v>33276</v>
       </c>
       <c r="Q27" t="n">
-        <v>109897</v>
+        <v>109898</v>
       </c>
       <c r="R27" t="n">
         <v>23756</v>
       </c>
       <c r="S27" t="n">
-        <v>27136</v>
+        <v>24055</v>
       </c>
       <c r="T27" t="n">
-        <v>25896</v>
+        <v>20279</v>
       </c>
       <c r="U27" t="n">
-        <v>13955</v>
+        <v>13152</v>
       </c>
       <c r="V27" t="n">
-        <v>44926</v>
+        <v>44927</v>
       </c>
       <c r="W27" t="n">
-        <v>43399</v>
+        <v>43398</v>
       </c>
       <c r="X27" t="n">
-        <v>97755</v>
+        <v>97753</v>
       </c>
       <c r="Y27" t="n">
         <v>82976</v>
       </c>
       <c r="Z27" t="n">
-        <v>16029</v>
+        <v>11676</v>
       </c>
       <c r="AA27" t="n">
         <v>0</v>
       </c>
       <c r="AB27" t="n">
-        <v>14251</v>
+        <v>10644</v>
       </c>
       <c r="AC27" t="n">
-        <v>24926</v>
+        <v>19308</v>
       </c>
       <c r="AD27" t="n">
-        <v>31235</v>
+        <v>27575</v>
       </c>
     </row>
     <row r="28">
@@ -3031,82 +3031,82 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>12500</v>
+        <v>7785</v>
       </c>
       <c r="C28" t="n">
-        <v>33737</v>
+        <v>33235</v>
       </c>
       <c r="D28" t="n">
-        <v>140489</v>
+        <v>135120</v>
       </c>
       <c r="E28" t="n">
-        <v>42076</v>
+        <v>34391</v>
       </c>
       <c r="F28" t="n">
-        <v>10154</v>
+        <v>8390</v>
       </c>
       <c r="G28" t="n">
-        <v>41588</v>
+        <v>41084</v>
       </c>
       <c r="H28" t="n">
-        <v>56224</v>
+        <v>55721</v>
       </c>
       <c r="I28" t="n">
         <v>10575</v>
       </c>
       <c r="J28" t="n">
-        <v>18045</v>
+        <v>17257</v>
       </c>
       <c r="K28" t="n">
-        <v>14348</v>
+        <v>13200</v>
       </c>
       <c r="L28" t="n">
-        <v>16929</v>
+        <v>16928</v>
       </c>
       <c r="M28" t="n">
-        <v>34772</v>
+        <v>32784</v>
       </c>
       <c r="N28" t="n">
-        <v>66599</v>
+        <v>60182</v>
       </c>
       <c r="O28" t="n">
-        <v>18517</v>
+        <v>16791</v>
       </c>
       <c r="P28" t="n">
-        <v>23709</v>
+        <v>23708</v>
       </c>
       <c r="Q28" t="n">
         <v>103644</v>
       </c>
       <c r="R28" t="n">
-        <v>18004</v>
+        <v>17502</v>
       </c>
       <c r="S28" t="n">
-        <v>14488</v>
+        <v>14014</v>
       </c>
       <c r="T28" t="n">
-        <v>9633</v>
+        <v>9635</v>
       </c>
       <c r="U28" t="n">
-        <v>9906</v>
+        <v>7823</v>
       </c>
       <c r="V28" t="n">
-        <v>61023</v>
+        <v>54523</v>
       </c>
       <c r="W28" t="n">
-        <v>37647</v>
+        <v>34136</v>
       </c>
       <c r="X28" t="n">
-        <v>92003</v>
+        <v>91499</v>
       </c>
       <c r="Y28" t="n">
-        <v>77224</v>
+        <v>76722</v>
       </c>
       <c r="Z28" t="n">
         <v>2564</v>
       </c>
       <c r="AA28" t="n">
-        <v>13476</v>
+        <v>9779</v>
       </c>
       <c r="AB28" t="n">
         <v>0</v>
@@ -3115,7 +3115,7 @@
         <v>8664</v>
       </c>
       <c r="AD28" t="n">
-        <v>37477</v>
+        <v>36556</v>
       </c>
     </row>
     <row r="29">
@@ -3125,91 +3125,91 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17390</v>
+        <v>15167</v>
       </c>
       <c r="C29" t="n">
-        <v>32607</v>
+        <v>32608</v>
       </c>
       <c r="D29" t="n">
-        <v>139359</v>
+        <v>132487</v>
       </c>
       <c r="E29" t="n">
-        <v>46966</v>
+        <v>41859</v>
       </c>
       <c r="F29" t="n">
-        <v>12932</v>
+        <v>12087</v>
       </c>
       <c r="G29" t="n">
-        <v>40458</v>
+        <v>38451</v>
       </c>
       <c r="H29" t="n">
-        <v>55094</v>
+        <v>52946</v>
       </c>
       <c r="I29" t="n">
         <v>6713</v>
       </c>
       <c r="J29" t="n">
-        <v>28559</v>
+        <v>24725</v>
       </c>
       <c r="K29" t="n">
         <v>19238</v>
       </c>
       <c r="L29" t="n">
-        <v>9586</v>
+        <v>9585</v>
       </c>
       <c r="M29" t="n">
-        <v>39662</v>
+        <v>37194</v>
       </c>
       <c r="N29" t="n">
-        <v>62399</v>
+        <v>52839</v>
       </c>
       <c r="O29" t="n">
-        <v>10600</v>
+        <v>10599</v>
       </c>
       <c r="P29" t="n">
-        <v>19509</v>
+        <v>18194</v>
       </c>
       <c r="Q29" t="n">
-        <v>103016</v>
+        <v>100072</v>
       </c>
       <c r="R29" t="n">
-        <v>16874</v>
+        <v>15092</v>
       </c>
       <c r="S29" t="n">
         <v>9365</v>
       </c>
       <c r="T29" t="n">
-        <v>2393</v>
+        <v>2394</v>
       </c>
       <c r="U29" t="n">
-        <v>10288</v>
+        <v>10289</v>
       </c>
       <c r="V29" t="n">
-        <v>71537</v>
+        <v>61991</v>
       </c>
       <c r="W29" t="n">
         <v>27673</v>
       </c>
       <c r="X29" t="n">
-        <v>90873</v>
+        <v>88866</v>
       </c>
       <c r="Y29" t="n">
-        <v>76094</v>
+        <v>74089</v>
       </c>
       <c r="Z29" t="n">
-        <v>9786</v>
+        <v>9110</v>
       </c>
       <c r="AA29" t="n">
-        <v>23990</v>
+        <v>17247</v>
       </c>
       <c r="AB29" t="n">
-        <v>8308</v>
+        <v>7468</v>
       </c>
       <c r="AC29" t="n">
         <v>0</v>
       </c>
       <c r="AD29" t="n">
-        <v>47991</v>
+        <v>44024</v>
       </c>
     </row>
     <row r="30">
@@ -3219,88 +3219,88 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>41320</v>
+        <v>40411</v>
       </c>
       <c r="C30" t="n">
-        <v>25432</v>
+        <v>25431</v>
       </c>
       <c r="D30" t="n">
-        <v>170228</v>
+        <v>147077</v>
       </c>
       <c r="E30" t="n">
-        <v>63111</v>
+        <v>56722</v>
       </c>
       <c r="F30" t="n">
-        <v>46789</v>
+        <v>44543</v>
       </c>
       <c r="G30" t="n">
-        <v>71328</v>
+        <v>52884</v>
       </c>
       <c r="H30" t="n">
-        <v>85964</v>
+        <v>67048</v>
       </c>
       <c r="I30" t="n">
-        <v>43686</v>
+        <v>41087</v>
       </c>
       <c r="J30" t="n">
-        <v>22647</v>
+        <v>21689</v>
       </c>
       <c r="K30" t="n">
         <v>45513</v>
       </c>
       <c r="L30" t="n">
-        <v>59303</v>
+        <v>50499</v>
       </c>
       <c r="M30" t="n">
-        <v>65539</v>
+        <v>65097</v>
       </c>
       <c r="N30" t="n">
-        <v>103234</v>
+        <v>87717</v>
       </c>
       <c r="O30" t="n">
-        <v>55152</v>
+        <v>53762</v>
       </c>
       <c r="P30" t="n">
-        <v>60345</v>
+        <v>60218</v>
       </c>
       <c r="Q30" t="n">
-        <v>133885</v>
+        <v>116109</v>
       </c>
       <c r="R30" t="n">
-        <v>47744</v>
+        <v>42578</v>
       </c>
       <c r="S30" t="n">
-        <v>51123</v>
+        <v>50997</v>
       </c>
       <c r="T30" t="n">
-        <v>49883</v>
+        <v>47221</v>
       </c>
       <c r="U30" t="n">
-        <v>37943</v>
+        <v>37942</v>
       </c>
       <c r="V30" t="n">
-        <v>28614</v>
+        <v>28613</v>
       </c>
       <c r="W30" t="n">
-        <v>67386</v>
+        <v>60125</v>
       </c>
       <c r="X30" t="n">
-        <v>121743</v>
+        <v>103964</v>
       </c>
       <c r="Y30" t="n">
-        <v>106963</v>
+        <v>88679</v>
       </c>
       <c r="Z30" t="n">
-        <v>40016</v>
+        <v>38618</v>
       </c>
       <c r="AA30" t="n">
-        <v>30275</v>
+        <v>27843</v>
       </c>
       <c r="AB30" t="n">
-        <v>38239</v>
+        <v>37586</v>
       </c>
       <c r="AC30" t="n">
-        <v>48914</v>
+        <v>46250</v>
       </c>
       <c r="AD30" t="n">
         <v>0</v>

</xml_diff>